<commit_message>
error handling for extracting output from llm
</commit_message>
<xml_diff>
--- a/files/output_one_sheet_split.xlsx
+++ b/files/output_one_sheet_split.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H28"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -478,7 +478,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>NET-33-06-12</t>
+          <t>NET-33-06-20</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -488,7 +488,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Ø261 x 23.6mm</t>
+          <t>Ø325 x 110mm</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -508,17 +508,17 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>"Part Number - Can be found on the middle right position of the page"</t>
+          <t>"Duxford Range - Can be found on the right side of the page"</t>
         </is>
       </c>
       <c r="H2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>NET-33-06-32</t>
+          <t>NET-33-06-30</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -532,17 +532,17 @@
       <c r="F3" t="inlineStr"/>
       <c r="G3" t="inlineStr">
         <is>
-          <t>"Part Number - Can be found on the middle right position of the page"</t>
+          <t>"Duxford Range - Can be found on the right side of the page"</t>
         </is>
       </c>
       <c r="H3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>NET-33-06-16</t>
+          <t>NET-33-06-24</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -564,17 +564,17 @@
       <c r="F4" t="inlineStr"/>
       <c r="G4" t="inlineStr">
         <is>
-          <t>"Part Number - Can be found on the middle right position of the page"</t>
+          <t>"Duxford Range - Can be found on the right side of the page"</t>
         </is>
       </c>
       <c r="H4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>NET-33-06-36</t>
+          <t>NET-33-06-34</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -588,17 +588,17 @@
       <c r="F5" t="inlineStr"/>
       <c r="G5" t="inlineStr">
         <is>
-          <t>"Part Number - Can be found on the middle right position of the page"</t>
+          <t>"Duxford Range - Can be found on the right side of the page"</t>
         </is>
       </c>
       <c r="H5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>NET-33-06-72</t>
+          <t>NET-33-06-70</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -620,17 +620,17 @@
       <c r="F6" t="inlineStr"/>
       <c r="G6" t="inlineStr">
         <is>
-          <t>"Part Number - Can be found on the middle right position of the page"</t>
+          <t>"Duxford Range - Can be found on the right side of the page"</t>
         </is>
       </c>
       <c r="H6" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>NET-33-06-73</t>
+          <t>NET-33-06-71</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -644,17 +644,17 @@
       <c r="F7" t="inlineStr"/>
       <c r="G7" t="inlineStr">
         <is>
-          <t>"Part Number - Can be found on the middle right position of the page"</t>
+          <t>"Duxford Range - Can be found on the right side of the page"</t>
         </is>
       </c>
       <c r="H7" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>NET-33-06-78</t>
+          <t>NET-33-06-48</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -676,17 +676,17 @@
       <c r="F8" t="inlineStr"/>
       <c r="G8" t="inlineStr">
         <is>
-          <t>"Part Number - Can be found on the middle right position of the page"</t>
+          <t>"Duxford Range - Can be found on the right side of the page"</t>
         </is>
       </c>
       <c r="H8" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>NET-33-06-79</t>
+          <t>NET-33-06-49</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -700,17 +700,17 @@
       <c r="F9" t="inlineStr"/>
       <c r="G9" t="inlineStr">
         <is>
-          <t>"Part Number - Can be found on the middle right position of the page"</t>
+          <t>"Duxford Range - Can be found on the right side of the page"</t>
         </is>
       </c>
       <c r="H9" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>NET-33-06-03</t>
+          <t>NET-33-06-40</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -720,7 +720,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Ø261 x 23.6mm</t>
+          <t>Ø325 x 110mm</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -740,17 +740,17 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>"Part Number - Can be found on the middle right position of the page"</t>
+          <t>"Duxford Range - Can be found on the right side of the page"</t>
         </is>
       </c>
       <c r="H10" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>NET-33-06-05</t>
+          <t>NET-33-06-42</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -764,17 +764,17 @@
       <c r="F11" t="inlineStr"/>
       <c r="G11" t="inlineStr">
         <is>
-          <t>"Part Number - Can be found on the middle right position of the page"</t>
+          <t>"Duxford Range - Can be found on the right side of the page"</t>
         </is>
       </c>
       <c r="H11" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>NET-33-06-07</t>
+          <t>NET-33-06-44</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -796,17 +796,17 @@
       <c r="F12" t="inlineStr"/>
       <c r="G12" t="inlineStr">
         <is>
-          <t>"Part Number - Can be found on the middle right position of the page"</t>
+          <t>"Duxford Range - Can be found on the right side of the page"</t>
         </is>
       </c>
       <c r="H12" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>NET-33-06-09</t>
+          <t>NET-33-06-46</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -820,404 +820,10 @@
       <c r="F13" t="inlineStr"/>
       <c r="G13" t="inlineStr">
         <is>
-          <t>"Part Number - Can be found on the middle right position of the page"</t>
+          <t>"Duxford Range - Can be found on the right side of the page"</t>
         </is>
       </c>
       <c r="H13" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="1" t="inlineStr">
-        <is>
-          <t>Part Number</t>
-        </is>
-      </c>
-      <c r="B16" s="1" t="inlineStr">
-        <is>
-          <t>Description</t>
-        </is>
-      </c>
-      <c r="C16" s="1" t="inlineStr">
-        <is>
-          <t>Dimensions</t>
-        </is>
-      </c>
-      <c r="D16" s="1" t="inlineStr">
-        <is>
-          <t>Power</t>
-        </is>
-      </c>
-      <c r="E16" s="1" t="inlineStr">
-        <is>
-          <t>Lumens</t>
-        </is>
-      </c>
-      <c r="F16" s="1" t="inlineStr">
-        <is>
-          <t>Colour Temp.</t>
-        </is>
-      </c>
-      <c r="G16" s="1" t="inlineStr">
-        <is>
-          <t>table_header_descriptor</t>
-        </is>
-      </c>
-      <c r="H16" s="1" t="inlineStr">
-        <is>
-          <t>page_number</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>NET-33-06-20</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>Standard</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>Ø325 x 110mm</t>
-        </is>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>12W/14W/16W/18W</t>
-        </is>
-      </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>1200lm/1400lm/1600lm/1800lm</t>
-        </is>
-      </c>
-      <c r="F17" t="inlineStr">
-        <is>
-          <t>3000K/4000K/5500K</t>
-        </is>
-      </c>
-      <c r="G17" t="inlineStr">
-        <is>
-          <t>"Part Number, Description, Dimensions, Power, Lumens, Colour Temp. - Can be found on the top right position of the page"</t>
-        </is>
-      </c>
-      <c r="H17" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>NET-33-06-30</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>Emergency/Self Test</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr"/>
-      <c r="D18" t="inlineStr"/>
-      <c r="E18" t="inlineStr"/>
-      <c r="F18" t="inlineStr"/>
-      <c r="G18" t="inlineStr">
-        <is>
-          <t>"Part Number, Description, Dimensions, Power, Lumens, Colour Temp. - Can be found on the top right position of the page"</t>
-        </is>
-      </c>
-      <c r="H18" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>NET-33-06-24</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>Microwave Sensor</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr"/>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>16W</t>
-        </is>
-      </c>
-      <c r="E19" t="inlineStr">
-        <is>
-          <t>1600lm</t>
-        </is>
-      </c>
-      <c r="F19" t="inlineStr"/>
-      <c r="G19" t="inlineStr">
-        <is>
-          <t>"Part Number, Description, Dimensions, Power, Lumens, Colour Temp. - Can be found on the top right position of the page"</t>
-        </is>
-      </c>
-      <c r="H19" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>NET-33-06-34</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>Microwave Sensor Emergency/Self Test</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr"/>
-      <c r="D20" t="inlineStr"/>
-      <c r="E20" t="inlineStr"/>
-      <c r="F20" t="inlineStr"/>
-      <c r="G20" t="inlineStr">
-        <is>
-          <t>"Part Number, Description, Dimensions, Power, Lumens, Colour Temp. - Can be found on the top right position of the page"</t>
-        </is>
-      </c>
-      <c r="H20" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>NET-33-06-70</t>
-        </is>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>Photocell</t>
-        </is>
-      </c>
-      <c r="C21" t="inlineStr"/>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>12W/14W/16W/18W</t>
-        </is>
-      </c>
-      <c r="E21" t="inlineStr">
-        <is>
-          <t>1200lm/1400lm/1600lm/1800lm</t>
-        </is>
-      </c>
-      <c r="F21" t="inlineStr"/>
-      <c r="G21" t="inlineStr">
-        <is>
-          <t>"Part Number, Description, Dimensions, Power, Lumens, Colour Temp. - Can be found on the top right position of the page"</t>
-        </is>
-      </c>
-      <c r="H21" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>NET-33-06-71</t>
-        </is>
-      </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>Photocell Emergency/Self Test</t>
-        </is>
-      </c>
-      <c r="C22" t="inlineStr"/>
-      <c r="D22" t="inlineStr"/>
-      <c r="E22" t="inlineStr"/>
-      <c r="F22" t="inlineStr"/>
-      <c r="G22" t="inlineStr">
-        <is>
-          <t>"Part Number, Description, Dimensions, Power, Lumens, Colour Temp. - Can be found on the top right position of the page"</t>
-        </is>
-      </c>
-      <c r="H22" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>NET-33-06-48</t>
-        </is>
-      </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>Photocell Microwave Sensor</t>
-        </is>
-      </c>
-      <c r="C23" t="inlineStr"/>
-      <c r="D23" t="inlineStr">
-        <is>
-          <t>16W</t>
-        </is>
-      </c>
-      <c r="E23" t="inlineStr">
-        <is>
-          <t>1600lm</t>
-        </is>
-      </c>
-      <c r="F23" t="inlineStr"/>
-      <c r="G23" t="inlineStr">
-        <is>
-          <t>"Part Number, Description, Dimensions, Power, Lumens, Colour Temp. - Can be found on the top right position of the page"</t>
-        </is>
-      </c>
-      <c r="H23" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>NET-33-06-49</t>
-        </is>
-      </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>Photocell Microwave Sensor Emergency/Self Test</t>
-        </is>
-      </c>
-      <c r="C24" t="inlineStr"/>
-      <c r="D24" t="inlineStr"/>
-      <c r="E24" t="inlineStr"/>
-      <c r="F24" t="inlineStr"/>
-      <c r="G24" t="inlineStr">
-        <is>
-          <t>"Part Number, Description, Dimensions, Power, Lumens, Colour Temp. - Can be found on the top right position of the page"</t>
-        </is>
-      </c>
-      <c r="H24" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>NET-33-06-40</t>
-        </is>
-      </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>Standard</t>
-        </is>
-      </c>
-      <c r="C25" t="inlineStr">
-        <is>
-          <t>Ø325 x 110mm</t>
-        </is>
-      </c>
-      <c r="D25" t="inlineStr">
-        <is>
-          <t>12W/14W/16W/18W</t>
-        </is>
-      </c>
-      <c r="E25" t="inlineStr">
-        <is>
-          <t>1200lm/1400lm/1600lm/1800lm</t>
-        </is>
-      </c>
-      <c r="F25" t="inlineStr">
-        <is>
-          <t>4000K</t>
-        </is>
-      </c>
-      <c r="G25" t="inlineStr">
-        <is>
-          <t>"Part Number, Description, Dimensions, Power, Lumens, Colour Temp. - Can be found on the top right position of the page"</t>
-        </is>
-      </c>
-      <c r="H25" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>NET-33-06-42</t>
-        </is>
-      </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>Emergency/Self Test</t>
-        </is>
-      </c>
-      <c r="C26" t="inlineStr"/>
-      <c r="D26" t="inlineStr"/>
-      <c r="E26" t="inlineStr"/>
-      <c r="F26" t="inlineStr"/>
-      <c r="G26" t="inlineStr">
-        <is>
-          <t>"Part Number, Description, Dimensions, Power, Lumens, Colour Temp. - Can be found on the top right position of the page"</t>
-        </is>
-      </c>
-      <c r="H26" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t>NET-33-06-44</t>
-        </is>
-      </c>
-      <c r="B27" t="inlineStr">
-        <is>
-          <t>Microwave Sensor</t>
-        </is>
-      </c>
-      <c r="C27" t="inlineStr"/>
-      <c r="D27" t="inlineStr">
-        <is>
-          <t>16W</t>
-        </is>
-      </c>
-      <c r="E27" t="inlineStr">
-        <is>
-          <t>1600lm</t>
-        </is>
-      </c>
-      <c r="F27" t="inlineStr"/>
-      <c r="G27" t="inlineStr">
-        <is>
-          <t>"Part Number, Description, Dimensions, Power, Lumens, Colour Temp. - Can be found on the top right position of the page"</t>
-        </is>
-      </c>
-      <c r="H27" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="inlineStr">
-        <is>
-          <t>NET-33-06-46</t>
-        </is>
-      </c>
-      <c r="B28" t="inlineStr">
-        <is>
-          <t>Microwave Sensor Emergency/Self Test</t>
-        </is>
-      </c>
-      <c r="C28" t="inlineStr"/>
-      <c r="D28" t="inlineStr"/>
-      <c r="E28" t="inlineStr"/>
-      <c r="F28" t="inlineStr"/>
-      <c r="G28" t="inlineStr">
-        <is>
-          <t>"Part Number, Description, Dimensions, Power, Lumens, Colour Temp. - Can be found on the top right position of the page"</t>
-        </is>
-      </c>
-      <c r="H28" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>